<commit_message>
updated gis data with Oceans
</commit_message>
<xml_diff>
--- a/results/soo_raninit/design_var_raninit.xlsx
+++ b/results/soo_raninit/design_var_raninit.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="20231112_160743" sheetId="1" r:id="rId1"/>
+    <sheet name="20231117_004323" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -444,31 +444,31 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9.911486273033445</v>
+        <v>9.887685873561283</v>
       </c>
       <c r="C2">
-        <v>63.744</v>
+        <v>67.508</v>
       </c>
       <c r="D2">
-        <v>44.576</v>
+        <v>45</v>
       </c>
       <c r="E2">
-        <v>6.225</v>
+        <v>6.398</v>
       </c>
       <c r="F2">
-        <v>15.74121577616071</v>
+        <v>53.80067879463388</v>
       </c>
       <c r="G2">
-        <v>26.48847145744032</v>
+        <v>23.12573499499788</v>
       </c>
       <c r="H2">
-        <v>5.613323765888673</v>
+        <v>15.58377651302141</v>
       </c>
       <c r="I2">
-        <v>0.03613444992658209</v>
+        <v>6.971449386839799E-14</v>
       </c>
       <c r="J2">
-        <v>0.5540490562874538</v>
+        <v>0.5540490632433228</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -476,7 +476,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>9.887685872833373</v>
+        <v>9.887685873337098</v>
       </c>
       <c r="C3">
         <v>67.508</v>
@@ -488,19 +488,19 @@
         <v>6.398</v>
       </c>
       <c r="F3">
-        <v>67.21857904759396</v>
+        <v>28.40732007142202</v>
       </c>
       <c r="G3">
-        <v>36.95455509574627</v>
+        <v>43.17340631793351</v>
       </c>
       <c r="H3">
-        <v>7.057649999735617</v>
+        <v>10.71805634781776</v>
       </c>
       <c r="I3">
-        <v>1.681790600475416E-10</v>
+        <v>3.977216486397376E-10</v>
       </c>
       <c r="J3">
-        <v>0.5540490630033926</v>
+        <v>0.5540490631557152</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -508,31 +508,31 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>9.89408055677049</v>
+        <v>9.887685872624445</v>
       </c>
       <c r="C4">
-        <v>65.084</v>
+        <v>67.508</v>
       </c>
       <c r="D4">
-        <v>44.249</v>
+        <v>45</v>
       </c>
       <c r="E4">
-        <v>6.507</v>
+        <v>6.398</v>
       </c>
       <c r="F4">
-        <v>30.43136734921717</v>
+        <v>82.07444463628691</v>
       </c>
       <c r="G4">
-        <v>41.53156933706114</v>
+        <v>12.41045808616558</v>
       </c>
       <c r="H4">
-        <v>2.998271690402884</v>
+        <v>8.097184146248848</v>
       </c>
       <c r="I4">
-        <v>2.385857478938065E-09</v>
+        <v>2.810586752793168E-11</v>
       </c>
       <c r="J4">
-        <v>0.5540490636866318</v>
+        <v>0.5540490629621135</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -540,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>9.887685874007779</v>
+        <v>9.88768587273287</v>
       </c>
       <c r="C5">
         <v>67.508</v>
@@ -552,19 +552,19 @@
         <v>6.398</v>
       </c>
       <c r="F5">
-        <v>8.373308064786528</v>
+        <v>96.56253840728907</v>
       </c>
       <c r="G5">
-        <v>22.26919382953024</v>
+        <v>26.41757907459404</v>
       </c>
       <c r="H5">
-        <v>19.65727114538753</v>
+        <v>6.055556448403865</v>
       </c>
       <c r="I5">
-        <v>2.901401828535578E-10</v>
+        <v>1.642667380451534E-10</v>
       </c>
       <c r="J5">
-        <v>0.5540490629621269</v>
+        <v>0.5540490629604622</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>9.887685872966374</v>
+        <v>9.887685873506896</v>
       </c>
       <c r="C6">
         <v>67.508</v>
@@ -584,19 +584,19 @@
         <v>6.398</v>
       </c>
       <c r="F6">
-        <v>65.99243059963695</v>
+        <v>78.64575117394067</v>
       </c>
       <c r="G6">
-        <v>30.04210774522885</v>
+        <v>40.12962747508074</v>
       </c>
       <c r="H6">
-        <v>15.71261638145089</v>
+        <v>2.543178722461228</v>
       </c>
       <c r="I6">
-        <v>3.447193965597685E-10</v>
+        <v>9.050511016641865E-11</v>
       </c>
       <c r="J6">
-        <v>0.5540490629809385</v>
+        <v>0.5540490633528374</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -604,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>9.887685878519946</v>
+        <v>9.887685874100129</v>
       </c>
       <c r="C7">
         <v>67.508</v>
@@ -616,19 +616,19 @@
         <v>6.398</v>
       </c>
       <c r="F7">
-        <v>83.38042569756864</v>
+        <v>53.26472933447988</v>
       </c>
       <c r="G7">
-        <v>28.44178707423309</v>
+        <v>35.59910158069809</v>
       </c>
       <c r="H7">
-        <v>16.12780991904862</v>
+        <v>8.356131243321208</v>
       </c>
       <c r="I7">
-        <v>6.117284995419866E-09</v>
+        <v>4.275206701666242E-13</v>
       </c>
       <c r="J7">
-        <v>0.5540490632842884</v>
+        <v>0.5540490636474353</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -636,7 +636,7 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>9.887685872954915</v>
+        <v>9.887685873501656</v>
       </c>
       <c r="C8">
         <v>67.508</v>
@@ -648,19 +648,19 @@
         <v>6.398</v>
       </c>
       <c r="F8">
-        <v>59.02489484393562</v>
+        <v>92.17888748638023</v>
       </c>
       <c r="G8">
-        <v>39.34454366924721</v>
+        <v>34.62169020381332</v>
       </c>
       <c r="H8">
-        <v>16.60779936696749</v>
+        <v>2.533066493887359</v>
       </c>
       <c r="I8">
-        <v>9.788745967848581E-11</v>
+        <v>8.606154219291573E-11</v>
       </c>
       <c r="J8">
-        <v>0.5540490629812991</v>
+        <v>0.5540490633515234</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -668,31 +668,31 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>9.911325286720585</v>
+        <v>9.887685873148341</v>
       </c>
       <c r="C9">
-        <v>63.744</v>
+        <v>67.508</v>
       </c>
       <c r="D9">
-        <v>44.567</v>
+        <v>45</v>
       </c>
       <c r="E9">
-        <v>6.229</v>
+        <v>6.398</v>
       </c>
       <c r="F9">
-        <v>37.28345666298405</v>
+        <v>60.58371469592151</v>
       </c>
       <c r="G9">
-        <v>39.74694353063505</v>
+        <v>12.2342866752645</v>
       </c>
       <c r="H9">
-        <v>19.94110692134081</v>
+        <v>6.676734214416083</v>
       </c>
       <c r="I9">
-        <v>0.03572372808093519</v>
+        <v>9.872658812097424E-10</v>
       </c>
       <c r="J9">
-        <v>0.5540490629618807</v>
+        <v>0.554049062959986</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -700,31 +700,31 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>9.897614238652519</v>
+        <v>9.887685872842852</v>
       </c>
       <c r="C10">
-        <v>63.797</v>
+        <v>67.508</v>
       </c>
       <c r="D10">
-        <v>43.845</v>
+        <v>45</v>
       </c>
       <c r="E10">
-        <v>6.567</v>
+        <v>6.398</v>
       </c>
       <c r="F10">
-        <v>6.065890942614426</v>
+        <v>75.15881692983167</v>
       </c>
       <c r="G10">
-        <v>39.11515048334331</v>
+        <v>29.78867235898434</v>
       </c>
       <c r="H10">
-        <v>13.89626457353218</v>
+        <v>4.694776253173051</v>
       </c>
       <c r="I10">
-        <v>-1.465607613418893E-15</v>
+        <v>2.222150258125098E-10</v>
       </c>
       <c r="J10">
-        <v>0.5540490630515666</v>
+        <v>0.5540490629515318</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -732,31 +732,31 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>9.896729472581217</v>
+        <v>9.88768587268456</v>
       </c>
       <c r="C11">
-        <v>64.116</v>
+        <v>67.508</v>
       </c>
       <c r="D11">
-        <v>43.945</v>
+        <v>45</v>
       </c>
       <c r="E11">
-        <v>6.552</v>
+        <v>6.398</v>
       </c>
       <c r="F11">
-        <v>38.7034584579527</v>
+        <v>40.80746988343155</v>
       </c>
       <c r="G11">
-        <v>22.19759411386104</v>
+        <v>16.96771891291861</v>
       </c>
       <c r="H11">
-        <v>4.76944321047651</v>
+        <v>4.633616952055194</v>
       </c>
       <c r="I11">
-        <v>-5.023113757774932E-15</v>
+        <v>7.867888506252839E-12</v>
       </c>
       <c r="J11">
-        <v>0.5540490630795482</v>
+        <v>0.5540490629602832</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -764,7 +764,7 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>9.88768587342541</v>
+        <v>9.887685872719308</v>
       </c>
       <c r="C12">
         <v>67.508</v>
@@ -776,19 +776,19 @@
         <v>6.398</v>
       </c>
       <c r="F12">
-        <v>70.8499689074457</v>
+        <v>69.78210060054715</v>
       </c>
       <c r="G12">
-        <v>16.66487508093768</v>
+        <v>10.11523867944968</v>
       </c>
       <c r="H12">
-        <v>13.07639473199474</v>
+        <v>1.399712997316497</v>
       </c>
       <c r="I12">
-        <v>1.433873240922668E-10</v>
+        <v>1.023248717040275E-12</v>
       </c>
       <c r="J12">
-        <v>0.5540490633024041</v>
+        <v>0.5540490629325576</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -796,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>9.88768587286663</v>
+        <v>9.887685872830188</v>
       </c>
       <c r="C13">
         <v>67.508</v>
@@ -808,19 +808,19 @@
         <v>6.398</v>
       </c>
       <c r="F13">
-        <v>34.17586082745191</v>
+        <v>47.0375902068889</v>
       </c>
       <c r="G13">
-        <v>37.41769367313578</v>
+        <v>10.26037631581632</v>
       </c>
       <c r="H13">
-        <v>14.39291244575075</v>
+        <v>18.24370378979914</v>
       </c>
       <c r="I13">
-        <v>1.262452534456286E-10</v>
+        <v>1.660216042825693E-10</v>
       </c>
       <c r="J13">
-        <v>0.5540490629312199</v>
+        <v>0.5540490629745497</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -828,31 +828,31 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>9.887685872714458</v>
+        <v>9.897762813813427</v>
       </c>
       <c r="C14">
-        <v>67.508</v>
+        <v>63.744</v>
       </c>
       <c r="D14">
-        <v>45</v>
+        <v>43.828</v>
       </c>
       <c r="E14">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F14">
-        <v>27.76806757186993</v>
+        <v>51.61707969696168</v>
       </c>
       <c r="G14">
-        <v>23.80462610509359</v>
+        <v>21.25838509691989</v>
       </c>
       <c r="H14">
-        <v>1.16931452970453</v>
+        <v>1.874085648312396</v>
       </c>
       <c r="I14">
-        <v>5.66340233081027E-11</v>
+        <v>2.76530266004262E-10</v>
       </c>
       <c r="J14">
-        <v>0.5540490629555723</v>
+        <v>0.5540490631116372</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B15">
-        <v>9.887685872964552</v>
+        <v>9.887685872843026</v>
       </c>
       <c r="C15">
         <v>67.508</v>
@@ -872,19 +872,19 @@
         <v>6.398</v>
       </c>
       <c r="F15">
-        <v>86.20400774330352</v>
+        <v>82.77377511404826</v>
       </c>
       <c r="G15">
-        <v>26.56324713386236</v>
+        <v>37.08522575130348</v>
       </c>
       <c r="H15">
-        <v>9.938574286671487</v>
+        <v>18.75231604516384</v>
       </c>
       <c r="I15">
-        <v>1.385056167687164E-15</v>
+        <v>2.144280861769048E-10</v>
       </c>
       <c r="J15">
-        <v>0.5540490630776678</v>
+        <v>0.5540490629706315</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
       <c r="B16">
-        <v>9.887685873081789</v>
+        <v>9.887685873144976</v>
       </c>
       <c r="C16">
         <v>67.508</v>
@@ -904,19 +904,19 @@
         <v>6.398</v>
       </c>
       <c r="F16">
-        <v>6.13927373108618</v>
+        <v>84.00726100692717</v>
       </c>
       <c r="G16">
-        <v>30.03777310295737</v>
+        <v>13.44996566044382</v>
       </c>
       <c r="H16">
-        <v>17.2176810580487</v>
+        <v>3.32195244175489</v>
       </c>
       <c r="I16">
-        <v>4.64070610046337E-10</v>
+        <v>4.760151800512461E-10</v>
       </c>
       <c r="J16">
-        <v>0.5540490629827615</v>
+        <v>0.5540490628863737</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -924,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>9.887685872934435</v>
+        <v>9.887685872712932</v>
       </c>
       <c r="C17">
         <v>67.508</v>
@@ -936,19 +936,19 @@
         <v>6.398</v>
       </c>
       <c r="F17">
-        <v>24.26882334290553</v>
+        <v>49.65657069353772</v>
       </c>
       <c r="G17">
-        <v>11.87724738627597</v>
+        <v>30.32461745550097</v>
       </c>
       <c r="H17">
-        <v>16.95081324532217</v>
+        <v>12.99558222199884</v>
       </c>
       <c r="I17">
-        <v>2.998897450284087E-10</v>
+        <v>8.933966237879969E-11</v>
       </c>
       <c r="J17">
-        <v>0.5540490630384254</v>
+        <v>0.554049062962362</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -956,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>9.887685873091684</v>
+        <v>9.887685872976036</v>
       </c>
       <c r="C18">
         <v>67.508</v>
@@ -968,19 +968,19 @@
         <v>6.398</v>
       </c>
       <c r="F18">
-        <v>76.95219400013478</v>
+        <v>67.09873712494755</v>
       </c>
       <c r="G18">
-        <v>11.53197000590015</v>
+        <v>31.77883856595626</v>
       </c>
       <c r="H18">
-        <v>10.06310030063961</v>
+        <v>17.0059774413178</v>
       </c>
       <c r="I18">
-        <v>3.487729942834964E-10</v>
+        <v>1.797370459935128E-10</v>
       </c>
       <c r="J18">
-        <v>0.5540490630361984</v>
+        <v>0.5540490630568248</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -988,31 +988,31 @@
         <v>1</v>
       </c>
       <c r="B19">
-        <v>9.896681318421368</v>
+        <v>9.887685872961256</v>
       </c>
       <c r="C19">
-        <v>64.133</v>
+        <v>67.508</v>
       </c>
       <c r="D19">
-        <v>43.951</v>
+        <v>45</v>
       </c>
       <c r="E19">
-        <v>6.551</v>
+        <v>6.398</v>
       </c>
       <c r="F19">
-        <v>43.24792315195031</v>
+        <v>9.041736164258156</v>
       </c>
       <c r="G19">
-        <v>15.0612555913464</v>
+        <v>12.26362139230347</v>
       </c>
       <c r="H19">
-        <v>15.04743118522886</v>
+        <v>12.25774675810869</v>
       </c>
       <c r="I19">
-        <v>5.882416736989002E-08</v>
+        <v>1.769829387547186E-10</v>
       </c>
       <c r="J19">
-        <v>0.554049062996692</v>
+        <v>0.5540490630496051</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1020,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="B20">
-        <v>9.887685873750877</v>
+        <v>9.887685872834588</v>
       </c>
       <c r="C20">
         <v>67.508</v>
@@ -1032,19 +1032,19 @@
         <v>6.398</v>
       </c>
       <c r="F20">
-        <v>65.19847348878723</v>
+        <v>69.0911151852669</v>
       </c>
       <c r="G20">
-        <v>28.10989752280794</v>
+        <v>15.18273977584165</v>
       </c>
       <c r="H20">
-        <v>13.915620547044</v>
+        <v>10.81138824169543</v>
       </c>
       <c r="I20">
-        <v>1.803066273450758E-09</v>
+        <v>1.845156436709992E-10</v>
       </c>
       <c r="J20">
-        <v>0.5540490629550647</v>
+        <v>0.5540490629885642</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
       <c r="B21">
-        <v>9.887685919985193</v>
+        <v>9.887685874420434</v>
       </c>
       <c r="C21">
         <v>67.508</v>
@@ -1064,19 +1064,19 @@
         <v>6.398</v>
       </c>
       <c r="F21">
-        <v>74.37871806513411</v>
+        <v>69.56380776904443</v>
       </c>
       <c r="G21">
-        <v>18.63006496506967</v>
+        <v>25.63339164123362</v>
       </c>
       <c r="H21">
-        <v>14.74386166917556</v>
+        <v>19.15050650031286</v>
       </c>
       <c r="I21">
-        <v>5.11207273881137E-08</v>
+        <v>2.800937223016766E-09</v>
       </c>
       <c r="J21">
-        <v>0.5540490629607761</v>
+        <v>0.554049062922472</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1084,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="B22">
-        <v>9.887685873206486</v>
+        <v>9.88768587417516</v>
       </c>
       <c r="C22">
         <v>67.508</v>
@@ -1096,19 +1096,19 @@
         <v>6.398</v>
       </c>
       <c r="F22">
-        <v>7.438082533303906</v>
+        <v>64.36852131576626</v>
       </c>
       <c r="G22">
-        <v>25.42872247679196</v>
+        <v>39.47633959696502</v>
       </c>
       <c r="H22">
-        <v>6.227019646186226</v>
+        <v>14.9080129813775</v>
       </c>
       <c r="I22">
-        <v>7.835601306674508E-10</v>
+        <v>1.093133576550909E-09</v>
       </c>
       <c r="J22">
-        <v>0.5540490630287302</v>
+        <v>0.5540490631309013</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1116,31 +1116,31 @@
         <v>1</v>
       </c>
       <c r="B23">
-        <v>9.887685872727241</v>
+        <v>9.897774353488511</v>
       </c>
       <c r="C23">
-        <v>67.508</v>
+        <v>63.743</v>
       </c>
       <c r="D23">
-        <v>45</v>
+        <v>43.828</v>
       </c>
       <c r="E23">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F23">
-        <v>26.47524477248285</v>
+        <v>59.71329851805187</v>
       </c>
       <c r="G23">
-        <v>36.75530245611695</v>
+        <v>25.32661505842508</v>
       </c>
       <c r="H23">
-        <v>3.130720183428367</v>
+        <v>2.597569580491221</v>
       </c>
       <c r="I23">
-        <v>1.311740527321398E-10</v>
+        <v>1.497717603707641E-07</v>
       </c>
       <c r="J23">
-        <v>0.5540490629702028</v>
+        <v>0.5540459695998747</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1148,7 +1148,7 @@
         <v>1</v>
       </c>
       <c r="B24">
-        <v>9.887685874017421</v>
+        <v>9.887685872864017</v>
       </c>
       <c r="C24">
         <v>67.508</v>
@@ -1160,19 +1160,19 @@
         <v>6.398</v>
       </c>
       <c r="F24">
-        <v>32.0050647088859</v>
+        <v>6.586757518339383</v>
       </c>
       <c r="G24">
-        <v>15.71961502943042</v>
+        <v>26.50913379329988</v>
       </c>
       <c r="H24">
-        <v>9.477434434748721</v>
+        <v>18.60101204648694</v>
       </c>
       <c r="I24">
-        <v>6.900657613488636E-13</v>
+        <v>1.828300303709817E-10</v>
       </c>
       <c r="J24">
-        <v>0.5540490636093868</v>
+        <v>0.5540490629782103</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1180,7 +1180,7 @@
         <v>1</v>
       </c>
       <c r="B25">
-        <v>9.887685872621271</v>
+        <v>9.887685873218382</v>
       </c>
       <c r="C25">
         <v>67.508</v>
@@ -1192,19 +1192,19 @@
         <v>6.398</v>
       </c>
       <c r="F25">
-        <v>83.73160336244786</v>
+        <v>73.33507562305067</v>
       </c>
       <c r="G25">
-        <v>41.6688954724174</v>
+        <v>42.09508064712423</v>
       </c>
       <c r="H25">
-        <v>15.57857615265674</v>
+        <v>8.010080821798473</v>
       </c>
       <c r="I25">
-        <v>9.458240773145368E-12</v>
+        <v>2.056192832609138E-12</v>
       </c>
       <c r="J25">
-        <v>0.5540490629602842</v>
+        <v>0.5540490630343501</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="B26">
-        <v>9.887685872821979</v>
+        <v>9.887685872757489</v>
       </c>
       <c r="C26">
         <v>67.508</v>
@@ -1224,19 +1224,19 @@
         <v>6.398</v>
       </c>
       <c r="F26">
-        <v>75.43862189065783</v>
+        <v>93.95258510208065</v>
       </c>
       <c r="G26">
-        <v>12.4903462988514</v>
+        <v>32.15755393837998</v>
       </c>
       <c r="H26">
-        <v>10.95838021734805</v>
+        <v>7.725897341852082</v>
       </c>
       <c r="I26">
-        <v>1.786219218586386E-10</v>
+        <v>1.409525492474358E-10</v>
       </c>
       <c r="J26">
-        <v>0.5540490629417549</v>
+        <v>0.5540490629429339</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1244,7 +1244,7 @@
         <v>1</v>
       </c>
       <c r="B27">
-        <v>9.887685872649426</v>
+        <v>9.887685873306891</v>
       </c>
       <c r="C27">
         <v>67.508</v>
@@ -1256,19 +1256,19 @@
         <v>6.398</v>
       </c>
       <c r="F27">
-        <v>75.3925131671468</v>
+        <v>61.96382432884861</v>
       </c>
       <c r="G27">
-        <v>23.2277858746086</v>
+        <v>21.11349998317779</v>
       </c>
       <c r="H27">
-        <v>8.57046390058985</v>
+        <v>16.69620905433381</v>
       </c>
       <c r="I27">
-        <v>7.692417276509963E-11</v>
+        <v>4.616853901122438E-15</v>
       </c>
       <c r="J27">
-        <v>0.55404906296239</v>
+        <v>0.5540490630824476</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1276,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>9.887685872738603</v>
+        <v>9.887685872985399</v>
       </c>
       <c r="C28">
         <v>67.508</v>
@@ -1288,19 +1288,19 @@
         <v>6.398</v>
       </c>
       <c r="F28">
-        <v>97.66346492469663</v>
+        <v>57.97452951180153</v>
       </c>
       <c r="G28">
-        <v>31.35139671483758</v>
+        <v>10.34003496691015</v>
       </c>
       <c r="H28">
-        <v>8.682243977388225</v>
+        <v>5.128189496676885</v>
       </c>
       <c r="I28">
-        <v>1.482878067488777E-10</v>
+        <v>2.308426946220971E-15</v>
       </c>
       <c r="J28">
-        <v>0.5540490629622767</v>
+        <v>0.5540490630846279</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1308,7 +1308,7 @@
         <v>1</v>
       </c>
       <c r="B29">
-        <v>9.887685873115894</v>
+        <v>9.887685873639571</v>
       </c>
       <c r="C29">
         <v>67.508</v>
@@ -1320,19 +1320,19 @@
         <v>6.398</v>
       </c>
       <c r="F29">
-        <v>68.29852500737206</v>
+        <v>67.03315708068192</v>
       </c>
       <c r="G29">
-        <v>44.69257300927024</v>
+        <v>44.97247940336046</v>
       </c>
       <c r="H29">
-        <v>4.53517611397443</v>
+        <v>9.891805943124169</v>
       </c>
       <c r="I29">
-        <v>8.337139376859131E-10</v>
+        <v>1.644731730862164E-09</v>
       </c>
       <c r="J29">
-        <v>0.55404906299043</v>
+        <v>0.5540490629625678</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1340,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="B30">
-        <v>9.887685873080592</v>
+        <v>9.887685872842715</v>
       </c>
       <c r="C30">
         <v>67.508</v>
@@ -1352,19 +1352,19 @@
         <v>6.398</v>
       </c>
       <c r="F30">
-        <v>50.57226471743216</v>
+        <v>70.33904863345292</v>
       </c>
       <c r="G30">
-        <v>43.76957434054857</v>
+        <v>28.54178111069897</v>
       </c>
       <c r="H30">
-        <v>10.4868216250649</v>
+        <v>19.81069111029944</v>
       </c>
       <c r="I30">
-        <v>3.745061067732304E-10</v>
+        <v>4.247257807170576E-10</v>
       </c>
       <c r="J30">
-        <v>0.5540490630140062</v>
+        <v>0.5540490629655935</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1372,7 +1372,7 @@
         <v>1</v>
       </c>
       <c r="B31">
-        <v>9.887685873579159</v>
+        <v>9.887685890497263</v>
       </c>
       <c r="C31">
         <v>67.508</v>
@@ -1384,19 +1384,19 @@
         <v>6.398</v>
       </c>
       <c r="F31">
-        <v>61.95128544428054</v>
+        <v>38.39206535659925</v>
       </c>
       <c r="G31">
-        <v>32.5044565982227</v>
+        <v>25.1381365220609</v>
       </c>
       <c r="H31">
-        <v>15.59007598699862</v>
+        <v>14.70619491458942</v>
       </c>
       <c r="I31">
-        <v>6.126809805870872E-10</v>
+        <v>1.138550447233656E-09</v>
       </c>
       <c r="J31">
-        <v>0.5540490632411271</v>
+        <v>0.5540490629632666</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="B32">
-        <v>9.887685873021592</v>
+        <v>9.887685873566674</v>
       </c>
       <c r="C32">
         <v>67.508</v>
@@ -1416,19 +1416,19 @@
         <v>6.398</v>
       </c>
       <c r="F32">
-        <v>26.43291630376833</v>
+        <v>90.32641561960907</v>
       </c>
       <c r="G32">
-        <v>25.56103815298746</v>
+        <v>35.65773582292505</v>
       </c>
       <c r="H32">
-        <v>7.774959886764662</v>
+        <v>16.70534166066291</v>
       </c>
       <c r="I32">
-        <v>6.462079579839309E-10</v>
+        <v>2.616217204043416E-15</v>
       </c>
       <c r="J32">
-        <v>0.5540490629557223</v>
+        <v>0.5540490634025528</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="B33">
-        <v>9.887685873755295</v>
+        <v>9.887685872745271</v>
       </c>
       <c r="C33">
         <v>67.508</v>
@@ -1448,19 +1448,19 @@
         <v>6.398</v>
       </c>
       <c r="F33">
-        <v>24.99974397821855</v>
+        <v>13.1260521607449</v>
       </c>
       <c r="G33">
-        <v>19.93524995673889</v>
+        <v>28.10014596497174</v>
       </c>
       <c r="H33">
-        <v>15.80989559766919</v>
+        <v>19.70477877815501</v>
       </c>
       <c r="I33">
-        <v>3.58575653833279E-14</v>
+        <v>1.877520582456983E-14</v>
       </c>
       <c r="J33">
-        <v>0.5540490631003382</v>
+        <v>0.5540490629942697</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="B34">
-        <v>9.887685872624036</v>
+        <v>9.887685872625068</v>
       </c>
       <c r="C34">
         <v>67.508</v>
@@ -1480,19 +1480,19 @@
         <v>6.398</v>
       </c>
       <c r="F34">
-        <v>59.41960095136719</v>
+        <v>10.5317451881236</v>
       </c>
       <c r="G34">
-        <v>34.01784654370712</v>
+        <v>38.82281550903215</v>
       </c>
       <c r="H34">
-        <v>14.9058656076505</v>
+        <v>12.02746144873218</v>
       </c>
       <c r="I34">
-        <v>1.603356408291804E-11</v>
+        <v>7.639508130947671E-12</v>
       </c>
       <c r="J34">
-        <v>0.5540490629615296</v>
+        <v>0.5540490629590156</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
       <c r="B35">
-        <v>9.88768587298366</v>
+        <v>9.887685872940533</v>
       </c>
       <c r="C35">
         <v>67.508</v>
@@ -1512,19 +1512,19 @@
         <v>6.398</v>
       </c>
       <c r="F35">
-        <v>10.15236476020666</v>
+        <v>85.96425496659498</v>
       </c>
       <c r="G35">
-        <v>34.35330195146849</v>
+        <v>40.81217939880281</v>
       </c>
       <c r="H35">
-        <v>6.210362872373148</v>
+        <v>11.37186948910995</v>
       </c>
       <c r="I35">
-        <v>6.18739831715924E-10</v>
+        <v>8.171831397526664E-14</v>
       </c>
       <c r="J35">
-        <v>0.5540490629505876</v>
+        <v>0.5540490629479722</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1532,31 +1532,31 @@
         <v>1</v>
       </c>
       <c r="B36">
-        <v>9.887685874186461</v>
+        <v>9.897762572859675</v>
       </c>
       <c r="C36">
-        <v>67.508</v>
+        <v>63.744</v>
       </c>
       <c r="D36">
-        <v>45</v>
+        <v>43.828</v>
       </c>
       <c r="E36">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F36">
-        <v>20.38504787155631</v>
+        <v>54.10262827597357</v>
       </c>
       <c r="G36">
-        <v>40.64711152017007</v>
+        <v>28.49521581839867</v>
       </c>
       <c r="H36">
-        <v>16.43788680614793</v>
+        <v>9.104431458550719</v>
       </c>
       <c r="I36">
-        <v>5.097549948081097E-10</v>
+        <v>3.539107259581901E-09</v>
       </c>
       <c r="J36">
-        <v>0.5540490634949021</v>
+        <v>0.5540490630034275</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>9.887685874123065</v>
+        <v>9.887685872863152</v>
       </c>
       <c r="C37">
         <v>67.508</v>
@@ -1576,19 +1576,19 @@
         <v>6.398</v>
       </c>
       <c r="F37">
-        <v>37.0048717418066</v>
+        <v>15.508340821521</v>
       </c>
       <c r="G37">
-        <v>14.27877044710208</v>
+        <v>33.06726363075508</v>
       </c>
       <c r="H37">
-        <v>6.109766191456981</v>
+        <v>11.46109832880008</v>
       </c>
       <c r="I37">
-        <v>1.811345675975942E-13</v>
+        <v>2.43126296064152E-10</v>
       </c>
       <c r="J37">
-        <v>0.55404906365803</v>
+        <v>0.5540490629765996</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="B38">
-        <v>9.88768587317254</v>
+        <v>9.887685873704383</v>
       </c>
       <c r="C38">
         <v>67.508</v>
@@ -1608,19 +1608,19 @@
         <v>6.398</v>
       </c>
       <c r="F38">
-        <v>31.43144676510438</v>
+        <v>23.44412182051167</v>
       </c>
       <c r="G38">
-        <v>20.37955191490985</v>
+        <v>29.64138321926259</v>
       </c>
       <c r="H38">
-        <v>13.19132205641035</v>
+        <v>9.820124229594784</v>
       </c>
       <c r="I38">
-        <v>7.999792018959134E-11</v>
+        <v>1.884885695152047E-09</v>
       </c>
       <c r="J38">
-        <v>0.5540490632018703</v>
+        <v>0.5540490629888991</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="B39">
-        <v>9.887685873308449</v>
+        <v>9.887685872610989</v>
       </c>
       <c r="C39">
         <v>67.508</v>
@@ -1640,19 +1640,19 @@
         <v>6.398</v>
       </c>
       <c r="F39">
-        <v>44.35165732514555</v>
+        <v>41.85976252349221</v>
       </c>
       <c r="G39">
-        <v>34.01499155413776</v>
+        <v>43.74352846959466</v>
       </c>
       <c r="H39">
-        <v>15.78880746996217</v>
+        <v>15.09918027483584</v>
       </c>
       <c r="I39">
-        <v>3.462640429991794E-14</v>
+        <v>1.656834965808675E-12</v>
       </c>
       <c r="J39">
-        <v>0.5540490629876506</v>
+        <v>0.5540490629619095</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1660,31 +1660,31 @@
         <v>1</v>
       </c>
       <c r="B40">
-        <v>9.88768587373977</v>
+        <v>9.919302086161268</v>
       </c>
       <c r="C40">
-        <v>67.508</v>
+        <v>63.745</v>
       </c>
       <c r="D40">
         <v>45</v>
       </c>
       <c r="E40">
-        <v>6.398</v>
+        <v>6.041</v>
       </c>
       <c r="F40">
-        <v>27.81272186614193</v>
+        <v>5.411217020913469</v>
       </c>
       <c r="G40">
-        <v>26.77316824244147</v>
+        <v>24.07774368330472</v>
       </c>
       <c r="H40">
-        <v>18.5351505182314</v>
+        <v>8.592495878838941</v>
       </c>
       <c r="I40">
-        <v>1.698491607678087E-09</v>
+        <v>0.05572901069401263</v>
       </c>
       <c r="J40">
-        <v>0.5540490629132213</v>
+        <v>0.5540490629603748</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1692,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>9.887685872895082</v>
+        <v>9.887685873866159</v>
       </c>
       <c r="C41">
         <v>67.508</v>
@@ -1704,19 +1704,19 @@
         <v>6.398</v>
       </c>
       <c r="F41">
-        <v>57.17722815498702</v>
+        <v>46.88491119692122</v>
       </c>
       <c r="G41">
-        <v>27.63291480436893</v>
+        <v>33.96587485331067</v>
       </c>
       <c r="H41">
-        <v>13.9964028973362</v>
+        <v>7.987273490448606</v>
       </c>
       <c r="I41">
-        <v>3.912760588016178E-10</v>
+        <v>1.341051402631146E-10</v>
       </c>
       <c r="J41">
-        <v>0.5540490629528401</v>
+        <v>0.5540490629620284</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1724,7 +1724,7 @@
         <v>1</v>
       </c>
       <c r="B42">
-        <v>9.887685872626287</v>
+        <v>9.887685873333286</v>
       </c>
       <c r="C42">
         <v>67.508</v>
@@ -1736,19 +1736,19 @@
         <v>6.398</v>
       </c>
       <c r="F42">
-        <v>92.36400769417095</v>
+        <v>10.65910010614258</v>
       </c>
       <c r="G42">
-        <v>37.67539045807887</v>
+        <v>42.52657974948013</v>
       </c>
       <c r="H42">
-        <v>13.7642265865893</v>
+        <v>1.835576922189788</v>
       </c>
       <c r="I42">
-        <v>1.749018148469017E-12</v>
+        <v>7.001445086964645E-10</v>
       </c>
       <c r="J42">
-        <v>0.5540490629577989</v>
+        <v>0.5540490629624565</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
       <c r="B43">
-        <v>9.887685872802489</v>
+        <v>9.887685874353624</v>
       </c>
       <c r="C43">
         <v>67.508</v>
@@ -1768,19 +1768,19 @@
         <v>6.398</v>
       </c>
       <c r="F43">
-        <v>21.30643870173974</v>
+        <v>23.4910081269325</v>
       </c>
       <c r="G43">
-        <v>17.07495704631422</v>
+        <v>24.66962941904172</v>
       </c>
       <c r="H43">
-        <v>1.155188547190425</v>
+        <v>16.54522773051592</v>
       </c>
       <c r="I43">
-        <v>5.406289737917169E-11</v>
+        <v>1.451457611743239E-09</v>
       </c>
       <c r="J43">
-        <v>0.5540490629339337</v>
+        <v>0.5540490631040172</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1788,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="B44">
-        <v>9.8876858773757</v>
+        <v>9.887685873004399</v>
       </c>
       <c r="C44">
         <v>67.508</v>
@@ -1800,19 +1800,19 @@
         <v>6.398</v>
       </c>
       <c r="F44">
-        <v>33.83373804934648</v>
+        <v>54.5090187625518</v>
       </c>
       <c r="G44">
-        <v>16.44633346777017</v>
+        <v>16.77867112298487</v>
       </c>
       <c r="H44">
-        <v>19.73878914445483</v>
+        <v>10.79699545275443</v>
       </c>
       <c r="I44">
-        <v>8.387168221191421E-09</v>
+        <v>1.84674155882726E-14</v>
       </c>
       <c r="J44">
-        <v>0.5540490630884294</v>
+        <v>0.5540490630135037</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
       <c r="B45">
-        <v>9.887685873082397</v>
+        <v>9.88768587348622</v>
       </c>
       <c r="C45">
         <v>67.508</v>
@@ -1832,19 +1832,19 @@
         <v>6.398</v>
       </c>
       <c r="F45">
-        <v>14.71436943612339</v>
+        <v>14.22604114925869</v>
       </c>
       <c r="G45">
-        <v>22.59774534054968</v>
+        <v>30.93716511784771</v>
       </c>
       <c r="H45">
-        <v>13.31619000148852</v>
+        <v>4.66302795587371</v>
       </c>
       <c r="I45">
-        <v>1.279899627075143E-11</v>
+        <v>1.267323314761968E-10</v>
       </c>
       <c r="J45">
-        <v>0.5540490630326735</v>
+        <v>0.5540490633344279</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -1852,31 +1852,31 @@
         <v>1</v>
       </c>
       <c r="B46">
-        <v>9.887685873377297</v>
+        <v>9.896828440475298</v>
       </c>
       <c r="C46">
-        <v>67.508</v>
+        <v>64.08</v>
       </c>
       <c r="D46">
-        <v>45</v>
+        <v>43.934</v>
       </c>
       <c r="E46">
-        <v>6.398</v>
+        <v>6.553</v>
       </c>
       <c r="F46">
-        <v>82.82728498573502</v>
+        <v>68.56143710155942</v>
       </c>
       <c r="G46">
-        <v>35.99527415012845</v>
+        <v>13.59127583653487</v>
       </c>
       <c r="H46">
-        <v>14.28445101969478</v>
+        <v>9.223705209555943</v>
       </c>
       <c r="I46">
-        <v>6.725267951080861E-10</v>
+        <v>1.462071605682278E-11</v>
       </c>
       <c r="J46">
-        <v>0.5540490631501356</v>
+        <v>0.5540490629632152</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -1884,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="B47">
-        <v>9.887685874119184</v>
+        <v>9.887685872783095</v>
       </c>
       <c r="C47">
         <v>67.508</v>
@@ -1896,19 +1896,19 @@
         <v>6.398</v>
       </c>
       <c r="F47">
-        <v>84.2768635591553</v>
+        <v>99.5888337888431</v>
       </c>
       <c r="G47">
-        <v>15.66644143362494</v>
+        <v>11.05283815810964</v>
       </c>
       <c r="H47">
-        <v>8.827916066237179</v>
+        <v>8.15390432458449</v>
       </c>
       <c r="I47">
-        <v>2.231479379919385E-14</v>
+        <v>1.706909363809165E-10</v>
       </c>
       <c r="J47">
-        <v>0.5540490636562838</v>
+        <v>0.5540490629672814</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -1916,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="B48">
-        <v>9.887685872733773</v>
+        <v>9.887685873103123</v>
       </c>
       <c r="C48">
         <v>67.508</v>
@@ -1928,19 +1928,19 @@
         <v>6.398</v>
       </c>
       <c r="F48">
-        <v>70.92568779552789</v>
+        <v>20.09502395229685</v>
       </c>
       <c r="G48">
-        <v>24.35936758770007</v>
+        <v>27.91274774127723</v>
       </c>
       <c r="H48">
-        <v>17.02241131875418</v>
+        <v>17.21888786031428</v>
       </c>
       <c r="I48">
-        <v>1.702212484069802E-10</v>
+        <v>8.464232143250633E-15</v>
       </c>
       <c r="J48">
-        <v>0.5540490629622922</v>
+        <v>0.5540490630717829</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -1948,31 +1948,31 @@
         <v>1</v>
       </c>
       <c r="B49">
-        <v>9.897762567451828</v>
+        <v>9.887685873105509</v>
       </c>
       <c r="C49">
-        <v>63.744</v>
+        <v>67.508</v>
       </c>
       <c r="D49">
-        <v>43.828</v>
+        <v>45</v>
       </c>
       <c r="E49">
-        <v>6.569</v>
+        <v>6.398</v>
       </c>
       <c r="F49">
-        <v>61.19213122376087</v>
+        <v>77.50002060533835</v>
       </c>
       <c r="G49">
-        <v>33.84978938259506</v>
+        <v>36.94755371580568</v>
       </c>
       <c r="H49">
-        <v>16.3281564554483</v>
+        <v>8.015976147316538</v>
       </c>
       <c r="I49">
-        <v>7.079464140335667E-08</v>
+        <v>6.155805196035436E-16</v>
       </c>
       <c r="J49">
-        <v>0.5540490634573464</v>
+        <v>0.5540490630606598</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -1980,7 +1980,7 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <v>9.887685873353465</v>
+        <v>9.887685873906699</v>
       </c>
       <c r="C50">
         <v>67.508</v>
@@ -1992,19 +1992,19 @@
         <v>6.398</v>
       </c>
       <c r="F50">
-        <v>78.33770648729592</v>
+        <v>72.35713569583524</v>
       </c>
       <c r="G50">
-        <v>43.53373684595277</v>
+        <v>20.64077007472716</v>
       </c>
       <c r="H50">
-        <v>3.517384687359042</v>
+        <v>13.3642884332044</v>
       </c>
       <c r="I50">
-        <v>6.266252642689665E-10</v>
+        <v>8.451498888539322E-10</v>
       </c>
       <c r="J50">
-        <v>0.5540490631497405</v>
+        <v>0.5540490629604182</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2012,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="B51">
-        <v>9.887685873920253</v>
+        <v>9.887685873951893</v>
       </c>
       <c r="C51">
         <v>67.508</v>
@@ -2024,19 +2024,19 @@
         <v>6.398</v>
       </c>
       <c r="F51">
-        <v>23.74342718178046</v>
+        <v>5.193507565769907</v>
       </c>
       <c r="G51">
-        <v>40.6408899097576</v>
+        <v>38.68997648965414</v>
       </c>
       <c r="H51">
-        <v>14.98481307033076</v>
+        <v>2.453503602676108</v>
       </c>
       <c r="I51">
-        <v>9.056990058074801E-11</v>
+        <v>6.171194698949471E-14</v>
       </c>
       <c r="J51">
-        <v>0.5540490629133918</v>
+        <v>0.5540490635794493</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2044,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="B52">
-        <v>9.887685872762933</v>
+        <v>9.887685873069627</v>
       </c>
       <c r="C52">
         <v>67.508</v>
@@ -2056,19 +2056,19 @@
         <v>6.398</v>
       </c>
       <c r="F52">
-        <v>84.8762622718891</v>
+        <v>6.156945062896537</v>
       </c>
       <c r="G52">
-        <v>39.73840400477187</v>
+        <v>35.89214419684129</v>
       </c>
       <c r="H52">
-        <v>19.70813282687851</v>
+        <v>10.53627021390791</v>
       </c>
       <c r="I52">
-        <v>1.358773957189901E-10</v>
+        <v>3.66270409436323E-14</v>
       </c>
       <c r="J52">
-        <v>0.55404906296571</v>
+        <v>0.5540490629849484</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2076,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="B53">
-        <v>9.887685882620957</v>
+        <v>9.887685880276925</v>
       </c>
       <c r="C53">
         <v>67.508</v>
@@ -2088,19 +2088,19 @@
         <v>6.398</v>
       </c>
       <c r="F53">
-        <v>23.562829416552</v>
+        <v>9.595040171517093</v>
       </c>
       <c r="G53">
-        <v>30.19127164192884</v>
+        <v>23.03427317343816</v>
       </c>
       <c r="H53">
-        <v>12.56046184106904</v>
+        <v>8.696630898752286</v>
       </c>
       <c r="I53">
-        <v>7.430980656757902E-12</v>
+        <v>8.458781111232353E-09</v>
       </c>
       <c r="J53">
-        <v>0.5540490629489211</v>
+        <v>0.5540490634622086</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="B54">
-        <v>9.887685872711165</v>
+        <v>9.887685874066571</v>
       </c>
       <c r="C54">
         <v>67.508</v>
@@ -2120,19 +2120,19 @@
         <v>6.398</v>
       </c>
       <c r="F54">
-        <v>93.85736702687073</v>
+        <v>42.34390087117387</v>
       </c>
       <c r="G54">
-        <v>42.65915325012086</v>
+        <v>34.57416342595737</v>
       </c>
       <c r="H54">
-        <v>8.838068533754548</v>
+        <v>4.711099389287073</v>
       </c>
       <c r="I54">
-        <v>4.968350365608098E-12</v>
+        <v>1.562636068573045E-09</v>
       </c>
       <c r="J54">
-        <v>0.5540490629353266</v>
+        <v>0.5540490630522088</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2140,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="B55">
-        <v>9.88768587298919</v>
+        <v>9.887685873483974</v>
       </c>
       <c r="C55">
         <v>67.508</v>
@@ -2152,19 +2152,19 @@
         <v>6.398</v>
       </c>
       <c r="F55">
-        <v>60.81231942380038</v>
+        <v>16.64137601738541</v>
       </c>
       <c r="G55">
-        <v>43.03461134409969</v>
+        <v>14.86359508709605</v>
       </c>
       <c r="H55">
-        <v>17.23234074793867</v>
+        <v>2.233546991021427</v>
       </c>
       <c r="I55">
-        <v>-3.077902595889282E-16</v>
+        <v>2.473094733469276E-13</v>
       </c>
       <c r="J55">
-        <v>0.5540490630623456</v>
+        <v>0.554049063364516</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2172,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="B56">
-        <v>9.887685872805715</v>
+        <v>9.887685873357878</v>
       </c>
       <c r="C56">
         <v>67.508</v>
@@ -2184,19 +2184,19 @@
         <v>6.398</v>
       </c>
       <c r="F56">
-        <v>2.247367465972943</v>
+        <v>89.11011292221805</v>
       </c>
       <c r="G56">
-        <v>43.41540670884714</v>
+        <v>20.4244318143633</v>
       </c>
       <c r="H56">
-        <v>6.432265654409988</v>
+        <v>11.57495862547467</v>
       </c>
       <c r="I56">
-        <v>1.939748078216616E-10</v>
+        <v>1.047506590746433E-09</v>
       </c>
       <c r="J56">
-        <v>0.5540490629717838</v>
+        <v>0.5540490629115158</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2204,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="B57">
-        <v>9.88768587323157</v>
+        <v>9.887685873013774</v>
       </c>
       <c r="C57">
         <v>67.508</v>
@@ -2216,19 +2216,19 @@
         <v>6.398</v>
       </c>
       <c r="F57">
-        <v>24.16473339589966</v>
+        <v>86.2413525140323</v>
       </c>
       <c r="G57">
-        <v>15.82936368684679</v>
+        <v>22.02448550164906</v>
       </c>
       <c r="H57">
-        <v>18.4847104873896</v>
+        <v>4.287764045813955</v>
       </c>
       <c r="I57">
-        <v>5.585931529850509E-10</v>
+        <v>8.039466200153355E-11</v>
       </c>
       <c r="J57">
-        <v>0.5540490629834424</v>
+        <v>0.5540490629622478</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2236,7 +2236,7 @@
         <v>1</v>
       </c>
       <c r="B58">
-        <v>9.887685872909641</v>
+        <v>9.887685872917785</v>
       </c>
       <c r="C58">
         <v>67.508</v>
@@ -2248,51 +2248,51 @@
         <v>6.398</v>
       </c>
       <c r="F58">
-        <v>52.65509277257389</v>
+        <v>41.14459875476598</v>
       </c>
       <c r="G58">
-        <v>42.32115630173671</v>
+        <v>10.99690604795845</v>
       </c>
       <c r="H58">
-        <v>2.309540998231733</v>
+        <v>7.901345445804033</v>
       </c>
       <c r="I58">
-        <v>2.797093229650966E-10</v>
+        <v>3.555400706512625E-10</v>
       </c>
       <c r="J58">
-        <v>0.5540490629799335</v>
+        <v>0.5540490629302475</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59">
-        <v>-887819.044625907</v>
+        <v>9.887685873274267</v>
       </c>
       <c r="C59">
-        <v>44.499</v>
+        <v>67.508</v>
       </c>
       <c r="D59">
-        <v>4.032</v>
+        <v>45</v>
       </c>
       <c r="E59">
-        <v>0.08699999999999999</v>
+        <v>6.398</v>
       </c>
       <c r="F59">
-        <v>32.87406289685866</v>
+        <v>32.28157753418789</v>
       </c>
       <c r="G59">
-        <v>32.56047378143887</v>
+        <v>35.00350515810895</v>
       </c>
       <c r="H59">
-        <v>13.10355584380865</v>
+        <v>8.598334842870681</v>
       </c>
       <c r="I59">
-        <v>0.9987813943683908</v>
+        <v>1.398906731223133E-13</v>
       </c>
       <c r="J59">
-        <v>0.4324949721519457</v>
+        <v>0.5540490631139692</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2300,31 +2300,31 @@
         <v>1</v>
       </c>
       <c r="B60">
-        <v>9.887685873025029</v>
+        <v>9.902942217669395</v>
       </c>
       <c r="C60">
-        <v>67.508</v>
+        <v>63.745</v>
       </c>
       <c r="D60">
-        <v>45</v>
+        <v>44.111</v>
       </c>
       <c r="E60">
-        <v>6.398</v>
+        <v>6.436</v>
       </c>
       <c r="F60">
-        <v>76.62735605264631</v>
+        <v>36.16197721923291</v>
       </c>
       <c r="G60">
-        <v>25.64710897096018</v>
+        <v>39.66742944337143</v>
       </c>
       <c r="H60">
-        <v>6.575307355872812</v>
+        <v>3.164183304221587</v>
       </c>
       <c r="I60">
-        <v>7.540321180925954E-10</v>
+        <v>0.0139126079445425</v>
       </c>
       <c r="J60">
-        <v>0.554049062968308</v>
+        <v>0.5540490630110017</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2332,7 +2332,7 @@
         <v>1</v>
       </c>
       <c r="B61">
-        <v>9.887685873936725</v>
+        <v>9.887685875259644</v>
       </c>
       <c r="C61">
         <v>67.508</v>
@@ -2344,19 +2344,19 @@
         <v>6.398</v>
       </c>
       <c r="F61">
-        <v>38.1099288430413</v>
+        <v>19.49692382139686</v>
       </c>
       <c r="G61">
-        <v>13.28058890646595</v>
+        <v>26.82417755685456</v>
       </c>
       <c r="H61">
-        <v>10.9565351454509</v>
+        <v>2.597591329230538</v>
       </c>
       <c r="I61">
-        <v>2.652747309086096E-10</v>
+        <v>4.588290998726571E-10</v>
       </c>
       <c r="J61">
-        <v>0.5540490629620339</v>
+        <v>0.554049063280405</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2364,31 +2364,31 @@
         <v>1</v>
       </c>
       <c r="B62">
-        <v>9.897674674015732</v>
+        <v>9.887685873130145</v>
       </c>
       <c r="C62">
-        <v>63.776</v>
+        <v>67.508</v>
       </c>
       <c r="D62">
-        <v>43.838</v>
+        <v>45</v>
       </c>
       <c r="E62">
-        <v>6.568</v>
+        <v>6.398</v>
       </c>
       <c r="F62">
-        <v>55.63226624577393</v>
+        <v>58.40447862660395</v>
       </c>
       <c r="G62">
-        <v>14.03172622874544</v>
+        <v>18.70776871736524</v>
       </c>
       <c r="H62">
-        <v>14.65768162545815</v>
+        <v>8.817170330570498</v>
       </c>
       <c r="I62">
-        <v>1.043838677679402E-07</v>
+        <v>7.340300606434435E-10</v>
       </c>
       <c r="J62">
-        <v>0.5540490629330257</v>
+        <v>0.55404906298441</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2396,31 +2396,31 @@
         <v>1</v>
       </c>
       <c r="B63">
-        <v>9.887685872791623</v>
+        <v>9.897762595935617</v>
       </c>
       <c r="C63">
-        <v>67.508</v>
+        <v>63.744</v>
       </c>
       <c r="D63">
-        <v>45</v>
+        <v>43.828</v>
       </c>
       <c r="E63">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F63">
-        <v>65.75177747764968</v>
+        <v>33.94884847047722</v>
       </c>
       <c r="G63">
-        <v>38.82538296989053</v>
+        <v>28.85960098880769</v>
       </c>
       <c r="H63">
-        <v>17.69537224819264</v>
+        <v>19.00577718657234</v>
       </c>
       <c r="I63">
-        <v>7.306632970790221E-11</v>
+        <v>2.193890344416304E-12</v>
       </c>
       <c r="J63">
-        <v>0.5540490629573347</v>
+        <v>0.5540490629682905</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2428,7 +2428,7 @@
         <v>1</v>
       </c>
       <c r="B64">
-        <v>9.887685872908865</v>
+        <v>9.887685872856343</v>
       </c>
       <c r="C64">
         <v>67.508</v>
@@ -2440,19 +2440,19 @@
         <v>6.398</v>
       </c>
       <c r="F64">
-        <v>89.58154716609721</v>
+        <v>4.975494517144501</v>
       </c>
       <c r="G64">
-        <v>31.25219948573879</v>
+        <v>20.4471979376377</v>
       </c>
       <c r="H64">
-        <v>11.5072274551433</v>
+        <v>2.831729453291487</v>
       </c>
       <c r="I64">
-        <v>1.489104664652764E-10</v>
+        <v>9.253637201732234E-11</v>
       </c>
       <c r="J64">
-        <v>0.5540490629232282</v>
+        <v>0.5540490629263451</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2460,7 +2460,7 @@
         <v>1</v>
       </c>
       <c r="B65">
-        <v>9.887685873013634</v>
+        <v>9.887685873202567</v>
       </c>
       <c r="C65">
         <v>67.508</v>
@@ -2472,19 +2472,19 @@
         <v>6.398</v>
       </c>
       <c r="F65">
-        <v>89.32242895593654</v>
+        <v>68.2878360794067</v>
       </c>
       <c r="G65">
-        <v>43.538807503257</v>
+        <v>17.31156198528149</v>
       </c>
       <c r="H65">
-        <v>9.7727322965179</v>
+        <v>18.28859880375849</v>
       </c>
       <c r="I65">
-        <v>7.113443793032349E-10</v>
+        <v>2.092973769498241E-14</v>
       </c>
       <c r="J65">
-        <v>0.5540490629599729</v>
+        <v>0.554049062996865</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2492,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="B66">
-        <v>9.88768587310431</v>
+        <v>9.887685872693204</v>
       </c>
       <c r="C66">
         <v>67.508</v>
@@ -2504,19 +2504,19 @@
         <v>6.398</v>
       </c>
       <c r="F66">
-        <v>71.98837507555294</v>
+        <v>2.430052082040732</v>
       </c>
       <c r="G66">
-        <v>35.48270791712888</v>
+        <v>44.61311970848669</v>
       </c>
       <c r="H66">
-        <v>8.340674533534635</v>
+        <v>19.48395628194703</v>
       </c>
       <c r="I66">
-        <v>8.106741442179438E-10</v>
+        <v>8.042667203628007E-11</v>
       </c>
       <c r="J66">
-        <v>0.5540490629622863</v>
+        <v>0.5540490629662916</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2524,7 +2524,7 @@
         <v>1</v>
       </c>
       <c r="B67">
-        <v>9.887685872738817</v>
+        <v>9.887685881120417</v>
       </c>
       <c r="C67">
         <v>67.508</v>
@@ -2536,19 +2536,19 @@
         <v>6.398</v>
       </c>
       <c r="F67">
-        <v>19.5908173635508</v>
+        <v>95.96575501031518</v>
       </c>
       <c r="G67">
-        <v>24.42007063893725</v>
+        <v>31.81670088401155</v>
       </c>
       <c r="H67">
-        <v>16.44355878680371</v>
+        <v>10.49314663767681</v>
       </c>
       <c r="I67">
-        <v>6.063468110412874E-14</v>
+        <v>5.390564986750731E-10</v>
       </c>
       <c r="J67">
-        <v>0.5540490629932013</v>
+        <v>0.5540490629687204</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="B68">
-        <v>9.887685874006896</v>
+        <v>9.887685872768913</v>
       </c>
       <c r="C68">
         <v>67.508</v>
@@ -2568,19 +2568,19 @@
         <v>6.398</v>
       </c>
       <c r="F68">
-        <v>20.6127915057778</v>
+        <v>58.95484149972111</v>
       </c>
       <c r="G68">
-        <v>20.84790158565636</v>
+        <v>24.24970665692432</v>
       </c>
       <c r="H68">
-        <v>2.008510644625782</v>
+        <v>8.083979993303362</v>
       </c>
       <c r="I68">
-        <v>2.537730687922114E-13</v>
+        <v>2.640117117678005E-11</v>
       </c>
       <c r="J68">
-        <v>0.5540490636046602</v>
+        <v>0.5540490629228406</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2588,7 +2588,7 @@
         <v>1</v>
       </c>
       <c r="B69">
-        <v>9.887685872740574</v>
+        <v>9.887685872630668</v>
       </c>
       <c r="C69">
         <v>67.508</v>
@@ -2600,19 +2600,19 @@
         <v>6.398</v>
       </c>
       <c r="F69">
-        <v>97.72848608179427</v>
+        <v>77.92585073102541</v>
       </c>
       <c r="G69">
-        <v>44.68773763749184</v>
+        <v>24.98691958391225</v>
       </c>
       <c r="H69">
-        <v>6.228626225275088</v>
+        <v>3.873891624546223</v>
       </c>
       <c r="I69">
-        <v>8.80587931855084E-13</v>
+        <v>4.036730808761202E-11</v>
       </c>
       <c r="J69">
-        <v>0.5540490629267992</v>
+        <v>0.554049062962168</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2620,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="B70">
-        <v>9.887685872631156</v>
+        <v>9.887685873086596</v>
       </c>
       <c r="C70">
         <v>67.508</v>
@@ -2632,19 +2632,19 @@
         <v>6.398</v>
       </c>
       <c r="F70">
-        <v>18.21881054990369</v>
+        <v>47.70195826456088</v>
       </c>
       <c r="G70">
-        <v>39.05629351909906</v>
+        <v>40.62023970179807</v>
       </c>
       <c r="H70">
-        <v>15.61944485473093</v>
+        <v>2.152184954398276</v>
       </c>
       <c r="I70">
-        <v>2.855554909676068E-11</v>
+        <v>4.770749022094675E-15</v>
       </c>
       <c r="J70">
-        <v>0.5540490629603539</v>
+        <v>0.5540490631326952</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2652,7 +2652,7 @@
         <v>1</v>
       </c>
       <c r="B71">
-        <v>9.887685872957105</v>
+        <v>9.887685881752855</v>
       </c>
       <c r="C71">
         <v>67.508</v>
@@ -2664,19 +2664,19 @@
         <v>6.398</v>
       </c>
       <c r="F71">
-        <v>14.33733181295204</v>
+        <v>95.26241664683518</v>
       </c>
       <c r="G71">
-        <v>12.16463380382506</v>
+        <v>39.35630904560618</v>
       </c>
       <c r="H71">
-        <v>1.942198121939271</v>
+        <v>2.663056543215813</v>
       </c>
       <c r="I71">
-        <v>1.83481468400481E-10</v>
+        <v>7.694756838910643E-16</v>
       </c>
       <c r="J71">
-        <v>0.554049063044586</v>
+        <v>0.5540490634708533</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2684,7 +2684,7 @@
         <v>1</v>
       </c>
       <c r="B72">
-        <v>9.887685872754604</v>
+        <v>9.887685872774041</v>
       </c>
       <c r="C72">
         <v>67.508</v>
@@ -2696,19 +2696,19 @@
         <v>6.398</v>
       </c>
       <c r="F72">
-        <v>71.43869858510112</v>
+        <v>1.784202178086745</v>
       </c>
       <c r="G72">
-        <v>27.98583899000506</v>
+        <v>36.75656852206838</v>
       </c>
       <c r="H72">
-        <v>11.87253100321416</v>
+        <v>18.04788794139972</v>
       </c>
       <c r="I72">
-        <v>1.753784281155913E-10</v>
+        <v>1.298874895466698E-12</v>
       </c>
       <c r="J72">
-        <v>0.5540490629621988</v>
+        <v>0.5540490629631322</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2716,7 +2716,7 @@
         <v>1</v>
       </c>
       <c r="B73">
-        <v>9.887685873376533</v>
+        <v>9.88768587366949</v>
       </c>
       <c r="C73">
         <v>67.508</v>
@@ -2728,19 +2728,19 @@
         <v>6.398</v>
       </c>
       <c r="F73">
-        <v>78.16114888642842</v>
+        <v>67.45351076743779</v>
       </c>
       <c r="G73">
-        <v>30.85922037603611</v>
+        <v>29.77621244736347</v>
       </c>
       <c r="H73">
-        <v>19.08974576372349</v>
+        <v>10.23135373841749</v>
       </c>
       <c r="I73">
-        <v>1.217646429392786E-09</v>
+        <v>7.469544810800121E-10</v>
       </c>
       <c r="J73">
-        <v>0.5540490629635654</v>
+        <v>0.5540490632660117</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2748,31 +2748,31 @@
         <v>1</v>
       </c>
       <c r="B74">
-        <v>9.897762819531581</v>
+        <v>9.887685913268479</v>
       </c>
       <c r="C74">
-        <v>63.744</v>
+        <v>67.508</v>
       </c>
       <c r="D74">
-        <v>43.828</v>
+        <v>45</v>
       </c>
       <c r="E74">
-        <v>6.569</v>
+        <v>6.398</v>
       </c>
       <c r="F74">
-        <v>61.13384120008459</v>
+        <v>99.12138281152528</v>
       </c>
       <c r="G74">
-        <v>40.86657230310279</v>
+        <v>36.80271041612544</v>
       </c>
       <c r="H74">
-        <v>17.85335223407484</v>
+        <v>6.378542356528826</v>
       </c>
       <c r="I74">
-        <v>6.091105187114407E-11</v>
+        <v>4.439102592983667E-08</v>
       </c>
       <c r="J74">
-        <v>0.5540490629593243</v>
+        <v>0.5540490630800811</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2780,10 +2780,10 @@
         <v>1</v>
       </c>
       <c r="B75">
-        <v>9.887686059993374</v>
+        <v>9.887685872630032</v>
       </c>
       <c r="C75">
-        <v>67.50700000000001</v>
+        <v>67.508</v>
       </c>
       <c r="D75">
         <v>45</v>
@@ -2792,19 +2792,19 @@
         <v>6.398</v>
       </c>
       <c r="F75">
-        <v>60.76075292785259</v>
+        <v>43.21774785092499</v>
       </c>
       <c r="G75">
-        <v>10.05697879992022</v>
+        <v>42.38963520269424</v>
       </c>
       <c r="H75">
-        <v>10.11230460767807</v>
+        <v>2.252820812182314</v>
       </c>
       <c r="I75">
-        <v>1.696397745064494E-08</v>
+        <v>3.983082966565347E-11</v>
       </c>
       <c r="J75">
-        <v>0.5540490629623106</v>
+        <v>0.5540490629622628</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2812,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="B76">
-        <v>9.887685872637451</v>
+        <v>9.887685872878661</v>
       </c>
       <c r="C76">
         <v>67.508</v>
@@ -2824,19 +2824,19 @@
         <v>6.398</v>
       </c>
       <c r="F76">
-        <v>15.44275111634994</v>
+        <v>72.37187442657124</v>
       </c>
       <c r="G76">
-        <v>13.86517118111304</v>
+        <v>31.55245828070942</v>
       </c>
       <c r="H76">
-        <v>14.81347976406282</v>
+        <v>18.35199639898086</v>
       </c>
       <c r="I76">
-        <v>3.452529507109273E-11</v>
+        <v>2.767585375664301E-10</v>
       </c>
       <c r="J76">
-        <v>0.5540490629596417</v>
+        <v>0.5540490630185002</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2844,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="B77">
-        <v>9.88768587344264</v>
+        <v>9.887685872846895</v>
       </c>
       <c r="C77">
         <v>67.508</v>
@@ -2856,19 +2856,19 @@
         <v>6.398</v>
       </c>
       <c r="F77">
-        <v>91.63964376123988</v>
+        <v>44.64220896051354</v>
       </c>
       <c r="G77">
-        <v>34.58108106709545</v>
+        <v>22.86210184830989</v>
       </c>
       <c r="H77">
-        <v>11.00394784505201</v>
+        <v>12.89381574653193</v>
       </c>
       <c r="I77">
-        <v>3.523479790331226E-10</v>
+        <v>6.042753825526275E-11</v>
       </c>
       <c r="J77">
-        <v>0.5540490629963299</v>
+        <v>0.5540490629205261</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -2876,31 +2876,31 @@
         <v>1</v>
       </c>
       <c r="B78">
-        <v>9.887685872832222</v>
+        <v>9.897736788471699</v>
       </c>
       <c r="C78">
-        <v>67.508</v>
+        <v>63.753</v>
       </c>
       <c r="D78">
-        <v>45</v>
+        <v>43.831</v>
       </c>
       <c r="E78">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F78">
-        <v>48.47707740460974</v>
+        <v>33.00040037515222</v>
       </c>
       <c r="G78">
-        <v>43.43724937445718</v>
+        <v>29.22587519215583</v>
       </c>
       <c r="H78">
-        <v>3.626211664081773</v>
+        <v>19.5566154166083</v>
       </c>
       <c r="I78">
-        <v>3.034224077295101E-10</v>
+        <v>8.682933988786615E-07</v>
       </c>
       <c r="J78">
-        <v>0.5540490629458044</v>
+        <v>0.5540490629630345</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2908,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="B79">
-        <v>9.887685872703829</v>
+        <v>9.887685873283116</v>
       </c>
       <c r="C79">
         <v>67.508</v>
@@ -2920,19 +2920,19 @@
         <v>6.398</v>
       </c>
       <c r="F79">
-        <v>94.64991341278207</v>
+        <v>31.54549004286987</v>
       </c>
       <c r="G79">
-        <v>31.60050085730131</v>
+        <v>26.42876712540605</v>
       </c>
       <c r="H79">
-        <v>4.02447228786622</v>
+        <v>14.60769172755455</v>
       </c>
       <c r="I79">
-        <v>2.75698508041809E-11</v>
+        <v>1.096138529410889E-09</v>
       </c>
       <c r="J79">
-        <v>0.5540490629623848</v>
+        <v>0.5540490629570592</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -2940,7 +2940,7 @@
         <v>1</v>
       </c>
       <c r="B80">
-        <v>9.887685876148545</v>
+        <v>9.887685872911792</v>
       </c>
       <c r="C80">
         <v>67.508</v>
@@ -2952,19 +2952,19 @@
         <v>6.398</v>
       </c>
       <c r="F80">
-        <v>96.03060017023881</v>
+        <v>71.88274162211384</v>
       </c>
       <c r="G80">
-        <v>37.32474075482374</v>
+        <v>18.61133408918212</v>
       </c>
       <c r="H80">
-        <v>3.165176741752574</v>
+        <v>7.526395602038084</v>
       </c>
       <c r="I80">
-        <v>6.599462837813544E-09</v>
+        <v>3.738520521282665E-10</v>
       </c>
       <c r="J80">
-        <v>0.5540490629640772</v>
+        <v>0.5540490629345122</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2972,7 +2972,7 @@
         <v>1</v>
       </c>
       <c r="B81">
-        <v>9.887685872694021</v>
+        <v>9.887685872764342</v>
       </c>
       <c r="C81">
         <v>67.508</v>
@@ -2984,19 +2984,19 @@
         <v>6.398</v>
       </c>
       <c r="F81">
-        <v>89.68143775637732</v>
+        <v>84.58220873059236</v>
       </c>
       <c r="G81">
-        <v>35.738801344015</v>
+        <v>32.25595863695167</v>
       </c>
       <c r="H81">
-        <v>3.728211654100201</v>
+        <v>12.34302333935796</v>
       </c>
       <c r="I81">
-        <v>7.952530827610188E-12</v>
+        <v>2.154531816249375E-15</v>
       </c>
       <c r="J81">
-        <v>0.5540490629701122</v>
+        <v>0.5540490629913768</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3004,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="B82">
-        <v>9.887685883315307</v>
+        <v>9.887685872776789</v>
       </c>
       <c r="C82">
         <v>67.508</v>
@@ -3016,19 +3016,19 @@
         <v>6.398</v>
       </c>
       <c r="F82">
-        <v>30.32916254022198</v>
+        <v>29.88571316525104</v>
       </c>
       <c r="G82">
-        <v>29.98846344351439</v>
+        <v>43.95311608786395</v>
       </c>
       <c r="H82">
-        <v>7.399937696042416</v>
+        <v>15.82519193468801</v>
       </c>
       <c r="I82">
-        <v>1.873765222378149E-08</v>
+        <v>1.837977228889444E-10</v>
       </c>
       <c r="J82">
-        <v>0.554049063057394</v>
+        <v>0.554049062962007</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3036,7 +3036,7 @@
         <v>1</v>
       </c>
       <c r="B83">
-        <v>9.887685873078269</v>
+        <v>9.887685874757176</v>
       </c>
       <c r="C83">
         <v>67.508</v>
@@ -3048,19 +3048,19 @@
         <v>6.398</v>
       </c>
       <c r="F83">
-        <v>60.03866445679962</v>
+        <v>95.22904844731731</v>
       </c>
       <c r="G83">
-        <v>22.92313128409543</v>
+        <v>44.15896588335285</v>
       </c>
       <c r="H83">
-        <v>8.744417391511872</v>
+        <v>5.317695524487449</v>
       </c>
       <c r="I83">
-        <v>4.720794664942649E-10</v>
+        <v>3.596682155892871E-09</v>
       </c>
       <c r="J83">
-        <v>0.5540490629795943</v>
+        <v>0.5540490629573868</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3068,7 +3068,7 @@
         <v>1</v>
       </c>
       <c r="B84">
-        <v>9.88768587267195</v>
+        <v>9.887685872742662</v>
       </c>
       <c r="C84">
         <v>67.508</v>
@@ -3080,19 +3080,19 @@
         <v>6.398</v>
       </c>
       <c r="F84">
-        <v>14.41339197894616</v>
+        <v>25.53213392501097</v>
       </c>
       <c r="G84">
-        <v>40.73562419611903</v>
+        <v>15.81785048229289</v>
       </c>
       <c r="H84">
-        <v>9.906156523281922</v>
+        <v>12.26202477073345</v>
       </c>
       <c r="I84">
-        <v>9.549177405332832E-11</v>
+        <v>2.06280108411563E-10</v>
       </c>
       <c r="J84">
-        <v>0.5540490629594236</v>
+        <v>0.5540490629733833</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3100,31 +3100,31 @@
         <v>1</v>
       </c>
       <c r="B85">
-        <v>9.887685872663377</v>
+        <v>9.897762695328883</v>
       </c>
       <c r="C85">
-        <v>67.508</v>
+        <v>63.744</v>
       </c>
       <c r="D85">
-        <v>45</v>
+        <v>43.828</v>
       </c>
       <c r="E85">
-        <v>6.398</v>
+        <v>6.569</v>
       </c>
       <c r="F85">
-        <v>67.77770683113158</v>
+        <v>48.27829182058609</v>
       </c>
       <c r="G85">
-        <v>37.39926983665325</v>
+        <v>34.24651670077301</v>
       </c>
       <c r="H85">
-        <v>2.624984977532555</v>
+        <v>18.82321282517719</v>
       </c>
       <c r="I85">
-        <v>3.221517527981277E-11</v>
+        <v>7.480842653858619E-14</v>
       </c>
       <c r="J85">
-        <v>0.5540490629521635</v>
+        <v>0.5540490630739922</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
       <c r="B86">
-        <v>9.887685872929309</v>
+        <v>9.887685873057336</v>
       </c>
       <c r="C86">
         <v>67.508</v>
@@ -3144,19 +3144,19 @@
         <v>6.398</v>
       </c>
       <c r="F86">
-        <v>18.41133024075656</v>
+        <v>42.06682909184107</v>
       </c>
       <c r="G86">
-        <v>31.09067641535407</v>
+        <v>33.02723247695327</v>
       </c>
       <c r="H86">
-        <v>10.96208689423968</v>
+        <v>1.798789289991543</v>
       </c>
       <c r="I86">
-        <v>1.538951297808364E-16</v>
+        <v>4.519456744283652E-10</v>
       </c>
       <c r="J86">
-        <v>0.5540490630419006</v>
+        <v>0.5540490629790359</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3164,7 +3164,7 @@
         <v>1</v>
       </c>
       <c r="B87">
-        <v>9.887685873550529</v>
+        <v>9.88768587344879</v>
       </c>
       <c r="C87">
         <v>67.508</v>
@@ -3176,19 +3176,19 @@
         <v>6.398</v>
       </c>
       <c r="F87">
-        <v>85.46030232855148</v>
+        <v>1.165639104967965</v>
       </c>
       <c r="G87">
-        <v>39.39549694163115</v>
+        <v>33.47102859600047</v>
       </c>
       <c r="H87">
-        <v>19.09811692323973</v>
+        <v>2.921676931699483</v>
       </c>
       <c r="I87">
-        <v>8.464232130728701E-14</v>
+        <v>4.914804099442536E-10</v>
       </c>
       <c r="J87">
-        <v>0.5540490633951193</v>
+        <v>0.55404906314247</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3196,7 +3196,7 @@
         <v>1</v>
       </c>
       <c r="B88">
-        <v>9.887685873243496</v>
+        <v>9.887685872755645</v>
       </c>
       <c r="C88">
         <v>67.508</v>
@@ -3208,19 +3208,19 @@
         <v>6.398</v>
       </c>
       <c r="F88">
-        <v>33.73045050428002</v>
+        <v>51.38035498768339</v>
       </c>
       <c r="G88">
-        <v>26.25194525511905</v>
+        <v>26.0760503606088</v>
       </c>
       <c r="H88">
-        <v>18.726101969217</v>
+        <v>5.351588396862852</v>
       </c>
       <c r="I88">
-        <v>1.89074325126477E-10</v>
+        <v>3.293355775824658E-14</v>
       </c>
       <c r="J88">
-        <v>0.5540490632076218</v>
+        <v>0.554049062998075</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3228,7 +3228,7 @@
         <v>1</v>
       </c>
       <c r="B89">
-        <v>9.887685873493634</v>
+        <v>9.887685874102871</v>
       </c>
       <c r="C89">
         <v>67.508</v>
@@ -3240,19 +3240,19 @@
         <v>6.398</v>
       </c>
       <c r="F89">
-        <v>4.097504327878999</v>
+        <v>82.9050294760488</v>
       </c>
       <c r="G89">
-        <v>21.29050002664336</v>
+        <v>29.56479732776924</v>
       </c>
       <c r="H89">
-        <v>17.81137577695329</v>
+        <v>7.21669949164049</v>
       </c>
       <c r="I89">
-        <v>1.332129631237777E-09</v>
+        <v>2.63217922740373E-10</v>
       </c>
       <c r="J89">
-        <v>0.5540490630344459</v>
+        <v>0.554049062963036</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3260,7 +3260,7 @@
         <v>1</v>
       </c>
       <c r="B90">
-        <v>9.887685872793122</v>
+        <v>9.887685873170671</v>
       </c>
       <c r="C90">
         <v>67.508</v>
@@ -3272,19 +3272,19 @@
         <v>6.398</v>
       </c>
       <c r="F90">
-        <v>23.91420611889402</v>
+        <v>38.9664119312192</v>
       </c>
       <c r="G90">
-        <v>20.4585198315263</v>
+        <v>42.67098385358881</v>
       </c>
       <c r="H90">
-        <v>17.20113768741125</v>
+        <v>6.812968578592708</v>
       </c>
       <c r="I90">
-        <v>7.25712490274141E-11</v>
+        <v>4.409095476457063E-13</v>
       </c>
       <c r="J90">
-        <v>0.5540490630245636</v>
+        <v>0.5540490630037844</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3292,7 +3292,7 @@
         <v>1</v>
       </c>
       <c r="B91">
-        <v>9.887685873178711</v>
+        <v>9.887685872986358</v>
       </c>
       <c r="C91">
         <v>67.508</v>
@@ -3304,19 +3304,19 @@
         <v>6.398</v>
       </c>
       <c r="F91">
-        <v>74.59554863842814</v>
+        <v>42.17353379286548</v>
       </c>
       <c r="G91">
-        <v>16.09604763517508</v>
+        <v>21.66469938970527</v>
       </c>
       <c r="H91">
-        <v>16.86798955482778</v>
+        <v>4.898014406484381</v>
       </c>
       <c r="I91">
-        <v>1.054966041575795E-09</v>
+        <v>7.001397365357244E-10</v>
       </c>
       <c r="J91">
-        <v>0.5540490629609512</v>
+        <v>0.554049062963807</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3324,31 +3324,31 @@
         <v>1</v>
       </c>
       <c r="B92">
-        <v>9.897745266826032</v>
+        <v>9.887685873525877</v>
       </c>
       <c r="C92">
-        <v>63.75</v>
+        <v>67.508</v>
       </c>
       <c r="D92">
-        <v>43.83</v>
+        <v>45</v>
       </c>
       <c r="E92">
-        <v>6.569</v>
+        <v>6.398</v>
       </c>
       <c r="F92">
-        <v>27.4102457110475</v>
+        <v>72.62962893204188</v>
       </c>
       <c r="G92">
-        <v>20.25929449394443</v>
+        <v>41.59473033263816</v>
       </c>
       <c r="H92">
-        <v>3.567880472417397</v>
+        <v>16.20140210981233</v>
       </c>
       <c r="I92">
-        <v>7.88263389635121E-13</v>
+        <v>9.311066262941449E-10</v>
       </c>
       <c r="J92">
-        <v>0.5540490630808342</v>
+        <v>0.5540490629909194</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -3356,7 +3356,7 @@
         <v>1</v>
       </c>
       <c r="B93">
-        <v>9.887685872629218</v>
+        <v>9.887685873011012</v>
       </c>
       <c r="C93">
         <v>67.508</v>
@@ -3368,19 +3368,19 @@
         <v>6.398</v>
       </c>
       <c r="F93">
-        <v>70.20885087618625</v>
+        <v>5.802174527155657</v>
       </c>
       <c r="G93">
-        <v>20.19381634545674</v>
+        <v>10.02797408098295</v>
       </c>
       <c r="H93">
-        <v>10.44592121774632</v>
+        <v>4.720549993154776</v>
       </c>
       <c r="I93">
-        <v>1.770101781229846E-12</v>
+        <v>7.518240307723827E-10</v>
       </c>
       <c r="J93">
-        <v>0.5540490629569792</v>
+        <v>0.5540490629624112</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -3388,7 +3388,7 @@
         <v>1</v>
       </c>
       <c r="B94">
-        <v>9.887685873378683</v>
+        <v>9.887685873463157</v>
       </c>
       <c r="C94">
         <v>67.508</v>
@@ -3400,19 +3400,19 @@
         <v>6.398</v>
       </c>
       <c r="F94">
-        <v>75.83155105100467</v>
+        <v>91.3990890182952</v>
       </c>
       <c r="G94">
-        <v>41.72552792390979</v>
+        <v>44.36473742425894</v>
       </c>
       <c r="H94">
-        <v>16.60189845024161</v>
+        <v>4.827027042026907</v>
       </c>
       <c r="I94">
-        <v>1.219988251270631E-09</v>
+        <v>9.931175900325894E-11</v>
       </c>
       <c r="J94">
-        <v>0.5540490629494998</v>
+        <v>0.5540490632963686</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -3420,7 +3420,7 @@
         <v>1</v>
       </c>
       <c r="B95">
-        <v>9.887685872990218</v>
+        <v>9.887685872885394</v>
       </c>
       <c r="C95">
         <v>67.508</v>
@@ -3432,19 +3432,19 @@
         <v>6.398</v>
       </c>
       <c r="F95">
-        <v>52.14668744004998</v>
+        <v>79.73756798722944</v>
       </c>
       <c r="G95">
-        <v>23.75138864750354</v>
+        <v>12.34111142605894</v>
       </c>
       <c r="H95">
-        <v>6.062606334396429</v>
+        <v>7.289494945590806</v>
       </c>
       <c r="I95">
-        <v>2.092973764288703E-14</v>
+        <v>3.072109980312311E-10</v>
       </c>
       <c r="J95">
-        <v>0.5540490630976878</v>
+        <v>0.5540490630141024</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -3452,7 +3452,7 @@
         <v>1</v>
       </c>
       <c r="B96">
-        <v>9.887685873485777</v>
+        <v>9.887685873316581</v>
       </c>
       <c r="C96">
         <v>67.508</v>
@@ -3464,19 +3464,19 @@
         <v>6.398</v>
       </c>
       <c r="F96">
-        <v>36.06188651513142</v>
+        <v>72.26105431676665</v>
       </c>
       <c r="G96">
-        <v>39.42168354951921</v>
+        <v>44.76416381984473</v>
       </c>
       <c r="H96">
-        <v>16.57614602720746</v>
+        <v>10.68579600830467</v>
       </c>
       <c r="I96">
-        <v>3.967142509036664E-10</v>
+        <v>9.013837817912692E-10</v>
       </c>
       <c r="J96">
-        <v>0.5540490632677958</v>
+        <v>0.5540490629716543</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -3484,7 +3484,7 @@
         <v>1</v>
       </c>
       <c r="B97">
-        <v>9.887685873557643</v>
+        <v>9.887685872609651</v>
       </c>
       <c r="C97">
         <v>67.508</v>
@@ -3496,19 +3496,19 @@
         <v>6.398</v>
       </c>
       <c r="F97">
-        <v>47.82877170286159</v>
+        <v>50.86213142432445</v>
       </c>
       <c r="G97">
-        <v>40.57578853352437</v>
+        <v>20.99370041075711</v>
       </c>
       <c r="H97">
-        <v>15.83511752230096</v>
+        <v>16.61453857847408</v>
       </c>
       <c r="I97">
-        <v>7.503781860293229E-10</v>
+        <v>1.263479014428534E-12</v>
       </c>
       <c r="J97">
-        <v>0.5540490632138066</v>
+        <v>0.5540490629624086</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -3516,7 +3516,7 @@
         <v>1</v>
       </c>
       <c r="B98">
-        <v>9.887685872862553</v>
+        <v>9.887685872680933</v>
       </c>
       <c r="C98">
         <v>67.508</v>
@@ -3528,19 +3528,19 @@
         <v>6.398</v>
       </c>
       <c r="F98">
-        <v>51.52706481014138</v>
+        <v>42.70247974029626</v>
       </c>
       <c r="G98">
-        <v>17.73962183540952</v>
+        <v>25.03684268230659</v>
       </c>
       <c r="H98">
-        <v>1.187343964891608</v>
+        <v>8.148465986432763</v>
       </c>
       <c r="I98">
-        <v>1.725727660941171E-10</v>
+        <v>3.319271715319258E-11</v>
       </c>
       <c r="J98">
-        <v>0.554049062972345</v>
+        <v>0.5540490629614551</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3548,7 +3548,7 @@
         <v>1</v>
       </c>
       <c r="B99">
-        <v>9.887685873902917</v>
+        <v>9.887685873051959</v>
       </c>
       <c r="C99">
         <v>67.508</v>
@@ -3560,19 +3560,19 @@
         <v>6.398</v>
       </c>
       <c r="F99">
-        <v>6.238739132653688</v>
+        <v>75.3098978269151</v>
       </c>
       <c r="G99">
-        <v>15.477478716022</v>
+        <v>24.36038613518124</v>
       </c>
       <c r="H99">
-        <v>6.71091450846931</v>
+        <v>13.3828434862303</v>
       </c>
       <c r="I99">
-        <v>1.820595390746094E-09</v>
+        <v>7.914920394166905E-10</v>
       </c>
       <c r="J99">
-        <v>0.554049063026024</v>
+        <v>0.5540490629585894</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -3580,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="B100">
-        <v>9.887685872619146</v>
+        <v>9.887685873105045</v>
       </c>
       <c r="C100">
         <v>67.508</v>
@@ -3592,19 +3592,19 @@
         <v>6.398</v>
       </c>
       <c r="F100">
-        <v>87.31554857762806</v>
+        <v>83.57036165473255</v>
       </c>
       <c r="G100">
-        <v>34.27048251491225</v>
+        <v>30.47478852312712</v>
       </c>
       <c r="H100">
-        <v>15.77781232075555</v>
+        <v>6.732671595414363</v>
       </c>
       <c r="I100">
-        <v>6.155805186359112E-16</v>
+        <v>6.646806058180303E-10</v>
       </c>
       <c r="J100">
-        <v>0.5540490629625567</v>
+        <v>0.5540490630270354</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -3612,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="B101">
-        <v>9.887685873956055</v>
+        <v>9.887685872782109</v>
       </c>
       <c r="C101">
         <v>67.508</v>
@@ -3624,19 +3624,19 @@
         <v>6.398</v>
       </c>
       <c r="F101">
-        <v>2.473376887462758</v>
+        <v>8.072930334118109</v>
       </c>
       <c r="G101">
-        <v>25.91795432691216</v>
+        <v>33.15191315551887</v>
       </c>
       <c r="H101">
-        <v>2.324228692759439</v>
+        <v>12.04728302057894</v>
       </c>
       <c r="I101">
-        <v>2.962193482135422E-10</v>
+        <v>1.764409201051752E-10</v>
       </c>
       <c r="J101">
-        <v>0.5540490629619483</v>
+        <v>0.5540490629586897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>